<commit_message>
Improve calc & excel export
</commit_message>
<xml_diff>
--- a/private/exports/tasks/task.xlsx
+++ b/private/exports/tasks/task.xlsx
@@ -13,14 +13,14 @@
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1"/>
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t xml:space="preserve">PROJET</t>
   </si>
@@ -43,8 +43,10 @@
     <t xml:space="preserve">OBSERVATEURS</t>
   </si>
   <si>
-    <t xml:space="preserve">{d.watchers[i].emails[i].address}
-{d.watchers[i+1].emails[i].address}</t>
+    <t xml:space="preserve">{d.watchers[i].emails[i].address}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{d.watchers[i+1].emails[i].address}</t>
   </si>
   <si>
     <t xml:space="preserve">DEBUT</t>
@@ -74,10 +76,31 @@
     <t xml:space="preserve">LISTE</t>
   </si>
   <si>
-    <t xml:space="preserve">{d.checklist[i].name}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{d.checklist[i+1].name}</t>
+    <t xml:space="preserve">{d.checklist[i, checked=true].name}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{d.checklist[i+1, checked=true].name}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{d.checklist[i, checked=false].name}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{d.checklist[i+1, checked=false].name}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DISCUSSION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{d.notes[i].createdBy.emails[i].address} ({d.notes[i].createdAt}) :</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{d.notes[i].content:convCRLF()}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{d.notes[i+1].createdBy.emails[i].address} ({d.notes[i+1].createdAt}) :</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{d.notes[i+1].content:convCRLF()}</t>
   </si>
 </sst>
 </file>
@@ -87,7 +110,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -113,6 +136,19 @@
       <color rgb="FF000000"/>
       <name val="Liberation Sans;Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <strike val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Liberation Sans;Arial"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Liberation Sans;Arial"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -215,11 +251,15 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -234,14 +274,34 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -321,112 +381,163 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="43.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="23.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="43.7"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="64" min="3" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="23.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="6"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="7" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
+      <c r="B5" s="7"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B6" s="7"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="s">
+      <c r="B7" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="4" t="s">
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="s">
+      <c r="B8" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="4" t="s">
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3" t="s">
+      <c r="B9" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="6"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="4"/>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="4" t="s">
+      <c r="B11" s="6"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="4"/>
+      <c r="B12" s="8"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="9"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="10"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="10"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="11"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>26</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
+  <mergeCells count="9">
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
     <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>